<commit_message>
Create new jar for extends package support.
</commit_message>
<xml_diff>
--- a/meta/objects/BlancoValueObjectArraySample.xlsx
+++ b/meta/objects/BlancoValueObjectArraySample.xlsx
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>クラス名</t>
   </si>
@@ -153,19 +153,15 @@
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>ArraySampleOya</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>パッケージ</t>
     <phoneticPr fontId="4"/>
   </si>
   <si>
-    <t>blanco.sample.myex</t>
-    <phoneticPr fontId="4"/>
-  </si>
-  <si>
     <t>blanco\sample\myex</t>
+    <phoneticPr fontId="4"/>
+  </si>
+  <si>
+    <t>PhpSample</t>
     <phoneticPr fontId="4"/>
   </si>
 </sst>
@@ -1035,7 +1031,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="12" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -1169,7 +1165,7 @@
       </c>
       <c r="B13" s="36"/>
       <c r="C13" s="37" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D13" s="37"/>
       <c r="E13" s="37"/>
@@ -1181,11 +1177,11 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.15">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="10" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D14" s="39"/>
       <c r="E14" s="11"/>
@@ -1197,7 +1193,7 @@
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D15" s="39"/>
       <c r="E15" s="11"/>

</xml_diff>